<commit_message>
update template download terima motor
</commit_message>
<xml_diff>
--- a/assets/excelTemplate/templateTerimaMotor.xlsx
+++ b/assets/excelTemplate/templateTerimaMotor.xlsx
@@ -15,9 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
-  <si>
-    <t>No Surat Jalan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>No.Polisi</t>
+  </si>
+  <si>
+    <t>Tanggal SJ</t>
+  </si>
+  <si>
+    <t>No.Surat Jalan</t>
   </si>
   <si>
     <t>No Sales Order</t>
@@ -395,15 +401,15 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,27 +434,33 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="J2">
+    <row r="2" spans="1:13">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>9</v>
+      <c r="M2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="J3">
+    <row r="3" spans="1:13">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="K3" t="s">
-        <v>10</v>
+      <c r="M3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix errorprint kwitansi dp
</commit_message>
<xml_diff>
--- a/assets/excelTemplate/templateTerimaMotor.xlsx
+++ b/assets/excelTemplate/templateTerimaMotor.xlsx
@@ -20,10 +20,10 @@
     <t>No.Polisi</t>
   </si>
   <si>
-    <t>Tanggal SJ</t>
-  </si>
-  <si>
     <t>No.Surat Jalan</t>
+  </si>
+  <si>
+    <t>NTanggal SJ</t>
   </si>
   <si>
     <t>No Sales Order</t>

</xml_diff>